<commit_message>
Project 3 reflection done
I still might proof read it a time or two more, but it is good enough to
submit
</commit_message>
<xml_diff>
--- a/Project Reflections/P3 Reflection/Submissions.xlsx
+++ b/Project Reflections/P3 Reflection/Submissions.xlsx
@@ -9,16 +9,6 @@
   <sheets>
     <sheet name="July18" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">July18!$A$2:$A$17</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">July18!$B$1</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">July18!$B$2:$B$17</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">July18!$C$1</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">July18!$C$2:$C$17</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">July18!$D$1</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">July18!$D$2:$D$17</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">July18!$D$2:$D$17</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -807,37 +797,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -859,6 +819,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-7E39-40AA-8108-5FE2DEA1AAFD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -874,6 +839,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7E39-40AA-8108-5FE2DEA1AAFD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -889,6 +859,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-7E39-40AA-8108-5FE2DEA1AAFD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1006,7 +981,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2539,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>